<commit_message>
ajustes servicio eliminar deudor
</commit_message>
<xml_diff>
--- a/migracion/Clientes.xlsx
+++ b/migracion/Clientes.xlsx
@@ -1,44 +1,109 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9FF69B-649F-4C3D-AECA-9C6358816167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>nit</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>contraseña</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>direccion</t>
+  </si>
+  <si>
+    <t>banco</t>
+  </si>
+  <si>
+    <t>numero_cuenta</t>
+  </si>
+  <si>
+    <t>tipo_cuenta</t>
+  </si>
+  <si>
+    <t>ejecutivoPrejuridico</t>
+  </si>
+  <si>
+    <t>ejecutivoJuridico</t>
+  </si>
+  <si>
+    <t>ejecutivoDependiente</t>
+  </si>
+  <si>
+    <t>abogado</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>EDIFICIO RESIDENCIAS LA CASTELLANA - P.H.</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>No tiene</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>90aUARGlIZOrm0aiVeGMJovUVGd2</t>
+  </si>
+  <si>
+    <t>mauruco009@gmail.com</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,17 +126,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,175 +472,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="3" max="3" width="36.08203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>nombre</v>
-      </c>
-      <c r="B1" t="str">
-        <v>nit</v>
-      </c>
-      <c r="C1" t="str">
-        <v>correo</v>
-      </c>
-      <c r="D1" t="str">
-        <v>contraseña</v>
-      </c>
-      <c r="E1" t="str">
-        <v>telefono</v>
-      </c>
-      <c r="F1" t="str">
-        <v>direccion</v>
-      </c>
-      <c r="G1" t="str">
-        <v>banco</v>
-      </c>
-      <c r="H1" t="str">
-        <v>numero_cuenta</v>
-      </c>
-      <c r="I1" t="str">
-        <v>tipo_cuenta</v>
-      </c>
-      <c r="J1" t="str">
-        <v>ejecutivoPrejuridico</v>
-      </c>
-      <c r="K1" t="str">
-        <v>ejecutivoJuridico</v>
-      </c>
-      <c r="L1" t="str">
-        <v>ejecutivoDependiente</v>
-      </c>
-      <c r="M1" t="str">
-        <v>abogado</v>
-      </c>
-      <c r="N1" t="str">
-        <v/>
-      </c>
-      <c r="O1" t="str">
-        <v/>
-      </c>
-      <c r="P1" t="str">
-        <v/>
-      </c>
-      <c r="Q1" t="str">
-        <v/>
-      </c>
-      <c r="R1" t="str">
-        <v/>
-      </c>
-      <c r="S1" t="str">
-        <v/>
-      </c>
-      <c r="T1" t="str">
-        <v/>
-      </c>
-      <c r="U1" t="str">
-        <v/>
-      </c>
-      <c r="V1" t="str">
-        <v/>
-      </c>
-      <c r="W1" t="str">
-        <v>UID</v>
-      </c>
-      <c r="X1" t="str">
-        <v>ERROR</v>
-      </c>
-      <c r="Y1" t="str">
-        <v/>
-      </c>
-      <c r="Z1" t="str">
-        <v/>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>EDIFICIO RESIDENCIAS LA CASTELLANA - P.H.</v>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
       </c>
       <c r="B2">
         <v>900087000</v>
       </c>
-      <c r="C2" t="str">
-        <v>edificiocastellanaph@gmail.com</v>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D2">
         <v>900087000</v>
       </c>
-      <c r="E2" t="str">
-        <v/>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <v/>
-      </c>
-      <c r="I2" t="str">
-        <v/>
-      </c>
-      <c r="J2" t="str">
-        <v>Jesus</v>
-      </c>
-      <c r="K2" t="str">
-        <v>No tiene</v>
-      </c>
-      <c r="L2" t="str">
-        <v>No tiene</v>
-      </c>
-      <c r="M2" t="str">
-        <v>Javier</v>
-      </c>
-      <c r="N2" t="str">
-        <v/>
-      </c>
-      <c r="O2" t="str">
-        <v/>
-      </c>
-      <c r="P2" t="str">
-        <v/>
-      </c>
-      <c r="Q2" t="str">
-        <v/>
-      </c>
-      <c r="R2" t="str">
-        <v/>
-      </c>
-      <c r="S2" t="str">
-        <v/>
-      </c>
-      <c r="T2" t="str">
-        <v/>
-      </c>
-      <c r="U2" t="str">
-        <v/>
-      </c>
-      <c r="V2" t="str">
-        <v/>
-      </c>
-      <c r="W2" t="str">
-        <v>90aUARGlIZOrm0aiVeGMJovUVGd2</v>
-      </c>
-      <c r="X2" t="str">
-        <v/>
-      </c>
-      <c r="Y2" t="str">
-        <v/>
-      </c>
-      <c r="Z2" t="str">
-        <v/>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{356D1A13-E562-40E9-88FF-2405B872F9D2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Z2"/>
+    <ignoredError sqref="A1:Z1 A2:B2 D2:Z2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajutes errores reportados jesus
</commit_message>
<xml_diff>
--- a/migracion/Clientes.xlsx
+++ b/migracion/Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9FF69B-649F-4C3D-AECA-9C6358816167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FC2C06-CE27-4080-8236-FAC589C8D696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>nombre</t>
   </si>
@@ -64,15 +64,6 @@
     <t/>
   </si>
   <si>
-    <t>UID</t>
-  </si>
-  <si>
-    <t>ERROR</t>
-  </si>
-  <si>
-    <t>EDIFICIO RESIDENCIAS LA CASTELLANA - P.H.</t>
-  </si>
-  <si>
     <t>Jesus</t>
   </si>
   <si>
@@ -82,10 +73,10 @@
     <t>Javier</t>
   </si>
   <si>
-    <t>90aUARGlIZOrm0aiVeGMJovUVGd2</t>
-  </si>
-  <si>
-    <t>mauruco009@gmail.com</t>
+    <t>CONJUNTO DE PRUEBA 1</t>
+  </si>
+  <si>
+    <t>santigarcia2321@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -473,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="T1" sqref="T1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -485,7 +476,7 @@
     <col min="3" max="3" width="36.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,65 +537,47 @@
       <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" t="s">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>111111</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>111111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="X1" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
-        <v>900087000</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2">
-        <v>900087000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
-      </c>
       <c r="N2" t="s">
         <v>13</v>
       </c>
@@ -624,34 +597,13 @@
         <v>13</v>
       </c>
       <c r="T2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" t="s">
-        <v>13</v>
-      </c>
-      <c r="V2" t="s">
-        <v>13</v>
-      </c>
-      <c r="W2" t="s">
-        <v>20</v>
-      </c>
-      <c r="X2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z2" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{356D1A13-E562-40E9-88FF-2405B872F9D2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Z1 A2:B2 D2:Z2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:S1 E2:S2 T1 T2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajuste reporte en word
</commit_message>
<xml_diff>
--- a/migracion/Clientes.xlsx
+++ b/migracion/Clientes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\DesarrolloWeb358\gestion-global\migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FC2C06-CE27-4080-8236-FAC589C8D696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711E56A4-2914-4063-B34E-6FBF116D7AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t>nombre</t>
   </si>
@@ -64,32 +64,171 @@
     <t/>
   </si>
   <si>
+    <t>AGRUPACION DE VIVIENDA LOS ROBLES - P.H.</t>
+  </si>
+  <si>
+    <t>agrupacionlosrobles2025@gmail.com</t>
+  </si>
+  <si>
+    <t>Nathaly P</t>
+  </si>
+  <si>
+    <t>laura</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>HLpR8m79wagEgKbtUMemjfYAnVG3</t>
+  </si>
+  <si>
+    <t>CONJUNTO RESIDENCIAL LOS ARRAYANES DE SUBA ETAPA I Y II -P.H.</t>
+  </si>
+  <si>
+    <t>crarrayanessuba@gmail.com</t>
+  </si>
+  <si>
+    <t>CARRERA 115 153-80</t>
+  </si>
+  <si>
+    <t>Iveth</t>
+  </si>
+  <si>
+    <t>No tiene</t>
+  </si>
+  <si>
+    <t>rZXaWDtMGSZ1coCIBcAI86MMHms1</t>
+  </si>
+  <si>
+    <t>CONJUNTO RESIDENCIAL ATALANTA ETAPA I - P.H.</t>
+  </si>
+  <si>
+    <t>atalantamicasa@gmail.com</t>
+  </si>
+  <si>
+    <t>4113919-3125125253</t>
+  </si>
+  <si>
+    <t>CALLE12 C # 71 C 31</t>
+  </si>
+  <si>
     <t>Jesus</t>
   </si>
   <si>
-    <t>No tiene</t>
-  </si>
-  <si>
-    <t>Javier</t>
-  </si>
-  <si>
-    <t>CONJUNTO DE PRUEBA 1</t>
-  </si>
-  <si>
-    <t>santigarcia2321@gmail.com</t>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>tDZpwcqcOyMCVGiECb3OH7CWSu43</t>
+  </si>
+  <si>
+    <t>CONJUNTO RESIDENCIAL BILBAO REAL - P.H.</t>
+  </si>
+  <si>
+    <t>admon.bilbaoreal@gmail.com</t>
+  </si>
+  <si>
+    <t>3182909644 - 3183271377</t>
+  </si>
+  <si>
+    <t>DIAGONAL 82G 73A - 61</t>
+  </si>
+  <si>
+    <t>LI2GgZa2jnU0zjfY7hqlLW0XRDK2</t>
+  </si>
+  <si>
+    <t>CONJUNTO RESIDENCIAL BOSQUES DE KENNEDY - P.H.</t>
+  </si>
+  <si>
+    <t>bosqueskennedy2024@gmail.com</t>
+  </si>
+  <si>
+    <t>3041026441-3123976697</t>
+  </si>
+  <si>
+    <t>CARRERA 78 K # 40 29 SUR</t>
+  </si>
+  <si>
+    <t>equfFlZBHaWVSPfDkdhrvdch0N92</t>
+  </si>
+  <si>
+    <t>CONJUNTO RESIDENCIAL CARABELAS CENTRAL - P.H.</t>
+  </si>
+  <si>
+    <t>admoncarabelascentral@gmail.com</t>
+  </si>
+  <si>
+    <t>CARRERA 40 C # 9 21 SUR</t>
+  </si>
+  <si>
+    <t>maTMi2632eVEJL3flzV7iaUJdZE2</t>
+  </si>
+  <si>
+    <t>CENTRO COMERCIAL CIUDAD MONTES - P.H.</t>
+  </si>
+  <si>
+    <t>ccciudadmontes@hotmail.com</t>
+  </si>
+  <si>
+    <t>2027145 - 3115836923</t>
+  </si>
+  <si>
+    <t>CALLE 11 SUR 31-39</t>
+  </si>
+  <si>
+    <t>sara</t>
+  </si>
+  <si>
+    <t>ecnQOGZORQfRxEQZ6HwzFzoTvdg1</t>
+  </si>
+  <si>
+    <t>CONJUNTO RESIDENCIAL PALO ROSA - P.H.</t>
+  </si>
+  <si>
+    <t>palorosaconjunto@gmail.com</t>
+  </si>
+  <si>
+    <t>9029213-3213648007</t>
+  </si>
+  <si>
+    <t>CRA 1 30-78 SUR</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>9Cdb2JGBTQRFPPxBjhdqLH0ljaz1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -99,16 +238,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Google Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF5E5E5E"/>
+      <name val="Google Sans"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C2F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6D9EEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,14 +283,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -464,19 +687,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:Y1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:Z9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="3" max="3" width="36.08203125" customWidth="1"/>
+    <col min="3" max="3" width="63.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="16" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,72 +761,411 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" ht="62.5" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5">
+        <v>830018673</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2">
+        <v>830018673</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
-        <v>111111</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2">
-        <v>111111</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+    </row>
+    <row r="3" spans="1:26" ht="62.5" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5">
+        <v>830074497</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2">
+        <v>830074497</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3004714483</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+    </row>
+    <row r="4" spans="1:26" ht="62.5" thickBot="1">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5">
+        <v>900122253</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2">
+        <v>900122253</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+    </row>
+    <row r="5" spans="1:26" ht="62.5" thickBot="1">
+      <c r="A5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5">
+        <v>900281120</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2">
+        <v>900281120</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" ht="62.5" thickBot="1">
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="5">
+        <v>860040335</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="2">
+        <v>860040335</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" ht="47" thickBot="1">
+      <c r="A7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="5">
+        <v>800193176</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2">
+        <v>800193176</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3202138789</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+    </row>
+    <row r="8" spans="1:26" ht="62.5" thickBot="1">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5">
+        <v>860450841</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="2">
+        <v>860450841</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" ht="47" thickBot="1">
+      <c r="A9" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="13">
+        <v>900643491</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2">
+        <v>900643491</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T2" t="s">
-        <v>13</v>
-      </c>
+      <c r="L9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="mailto:atalantamicasa@gmail.com" xr:uid="{3D5F424F-5DEE-4738-ABCD-9E0DDA23AE07}"/>
+    <hyperlink ref="C7" r:id="rId2" display="mailto:admoncarabelascentral@gmail.com" xr:uid="{C79A88E0-B1B6-4D26-A7D9-A072BD4A2E57}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:S1 E2:S2 T1 T2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:S1 T1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>